<commit_message>
MF changes to _site.yml, index.Rmd, R/ scipts, etc.
Former-commit-id: d1284ac216a630c660b9dc445113e012d9d7367f
</commit_message>
<xml_diff>
--- a/figureinfo/TOGS-lof4.xlsx
+++ b/figureinfo/TOGS-lof4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\friendly\Dropbox\Documents\DataVisHistory\figureinfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\friendly\Dropbox\DVH Website Templating Code\figureinfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4DE91F-5778-4DC6-865E-4B698934C0B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7689399B-7ABF-43E5-BA15-7B3196C31D84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2010" windowWidth="23940" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4620" yWindow="1410" windowWidth="23940" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="637">
   <si>
     <t>chapter</t>
   </si>
@@ -757,9 +757,6 @@
     <t>09_13-randu-2d.png</t>
   </si>
   <si>
-    <t>09_14a-randu0.pdf, 09_14b-randu1.pdf</t>
-  </si>
-  <si>
     <t>09_15-diabetes1.png</t>
   </si>
   <si>
@@ -1642,9 +1639,6 @@
     <t>© The Authors.</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Wikimedia Commons.</t>
   </si>
   <si>
@@ -1928,6 +1922,15 @@
   </si>
   <si>
     <t>07_4-minard-rhone.jpg</t>
+  </si>
+  <si>
+    <t>P_17-Minard-cotton3.png</t>
+  </si>
+  <si>
+    <t>09_14-randu-combined.png</t>
+  </si>
+  <si>
+    <t>Various sources</t>
   </si>
 </sst>
 </file>
@@ -2281,14 +2284,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2328,13 +2332,13 @@
         <v>150</v>
       </c>
       <c r="E2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2351,13 +2355,13 @@
         <v>151</v>
       </c>
       <c r="E3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G3" t="s">
-        <v>540</v>
+        <v>636</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2374,13 +2378,13 @@
         <v>152</v>
       </c>
       <c r="E4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G4" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2397,13 +2401,13 @@
         <v>153</v>
       </c>
       <c r="E5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G5" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2420,13 +2424,13 @@
         <v>154</v>
       </c>
       <c r="E6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G6" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2443,13 +2447,13 @@
         <v>155</v>
       </c>
       <c r="E7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F7" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G7" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2466,13 +2470,13 @@
         <v>156</v>
       </c>
       <c r="E8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G8" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2489,13 +2493,13 @@
         <v>157</v>
       </c>
       <c r="E9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G9" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2512,13 +2516,13 @@
         <v>158</v>
       </c>
       <c r="E10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G10" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2535,13 +2539,13 @@
         <v>159</v>
       </c>
       <c r="E11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F11" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G11" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2558,13 +2562,13 @@
         <v>160</v>
       </c>
       <c r="E12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G12" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2581,13 +2585,13 @@
         <v>161</v>
       </c>
       <c r="E13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F13" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G13" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2604,13 +2608,13 @@
         <v>162</v>
       </c>
       <c r="E14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G14" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2627,13 +2631,13 @@
         <v>163</v>
       </c>
       <c r="E15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F15" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G15" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2650,13 +2654,13 @@
         <v>164</v>
       </c>
       <c r="E16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G16" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2673,13 +2677,13 @@
         <v>165</v>
       </c>
       <c r="E17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F17" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G17" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2696,13 +2700,13 @@
         <v>166</v>
       </c>
       <c r="E18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F18" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G18" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2719,13 +2723,13 @@
         <v>167</v>
       </c>
       <c r="E19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F19" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G19" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2742,13 +2746,13 @@
         <v>168</v>
       </c>
       <c r="E20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F20" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G20" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2765,13 +2769,13 @@
         <v>169</v>
       </c>
       <c r="E21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F21" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G21" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2788,13 +2792,13 @@
         <v>170</v>
       </c>
       <c r="E22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F22" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G22" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2811,13 +2815,13 @@
         <v>171</v>
       </c>
       <c r="E23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G23" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2834,13 +2838,13 @@
         <v>172</v>
       </c>
       <c r="E24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G24" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2857,13 +2861,13 @@
         <v>173</v>
       </c>
       <c r="E25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F25" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G25" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2880,13 +2884,13 @@
         <v>174</v>
       </c>
       <c r="E26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F26" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G26" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2903,13 +2907,13 @@
         <v>175</v>
       </c>
       <c r="E27" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G27" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2926,13 +2930,13 @@
         <v>176</v>
       </c>
       <c r="E28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F28" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G28" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2949,13 +2953,13 @@
         <v>177</v>
       </c>
       <c r="E29" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F29" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G29" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2972,13 +2976,13 @@
         <v>178</v>
       </c>
       <c r="E30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G30" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2995,13 +2999,13 @@
         <v>179</v>
       </c>
       <c r="E31" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F31" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G31" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3018,13 +3022,13 @@
         <v>180</v>
       </c>
       <c r="E32" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F32" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -3041,13 +3045,13 @@
         <v>181</v>
       </c>
       <c r="E33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F33" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G33" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3064,13 +3068,13 @@
         <v>182</v>
       </c>
       <c r="E34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F34" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G34" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3087,13 +3091,13 @@
         <v>183</v>
       </c>
       <c r="E35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F35" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G35" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3110,13 +3114,13 @@
         <v>184</v>
       </c>
       <c r="E36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F36" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G36" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3133,13 +3137,13 @@
         <v>185</v>
       </c>
       <c r="E37" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F37" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G37" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3156,13 +3160,13 @@
         <v>186</v>
       </c>
       <c r="E38" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G38" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3179,13 +3183,13 @@
         <v>187</v>
       </c>
       <c r="E39" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F39" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G39" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3202,13 +3206,13 @@
         <v>188</v>
       </c>
       <c r="E40" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F40" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G40" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3225,13 +3229,13 @@
         <v>189</v>
       </c>
       <c r="E41" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F41" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G41" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3248,13 +3252,13 @@
         <v>190</v>
       </c>
       <c r="E42" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F42" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G42" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3271,13 +3275,13 @@
         <v>191</v>
       </c>
       <c r="E43" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F43" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G43" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3294,13 +3298,13 @@
         <v>192</v>
       </c>
       <c r="E44" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F44" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G44" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3317,13 +3321,13 @@
         <v>193</v>
       </c>
       <c r="E45" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F45" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G45" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3340,13 +3344,13 @@
         <v>194</v>
       </c>
       <c r="E46" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F46" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G46" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3363,13 +3367,13 @@
         <v>195</v>
       </c>
       <c r="E47" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F47" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G47" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3386,13 +3390,13 @@
         <v>196</v>
       </c>
       <c r="E48" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F48" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G48" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3409,13 +3413,13 @@
         <v>197</v>
       </c>
       <c r="E49" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F49" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G49" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3432,13 +3436,13 @@
         <v>198</v>
       </c>
       <c r="E50" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F50" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G50" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3455,13 +3459,13 @@
         <v>199</v>
       </c>
       <c r="E51" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F51" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G51" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3478,13 +3482,13 @@
         <v>200</v>
       </c>
       <c r="E52" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F52" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G52" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3501,13 +3505,13 @@
         <v>201</v>
       </c>
       <c r="E53" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F53" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G53" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3524,13 +3528,13 @@
         <v>202</v>
       </c>
       <c r="E54" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F54" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G54" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3547,13 +3551,13 @@
         <v>203</v>
       </c>
       <c r="E55" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F55" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G55" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3570,13 +3574,13 @@
         <v>204</v>
       </c>
       <c r="E56" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F56" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G56" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3593,13 +3597,13 @@
         <v>205</v>
       </c>
       <c r="E57" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F57" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G57" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3616,13 +3620,13 @@
         <v>206</v>
       </c>
       <c r="E58" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F58" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G58" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3639,13 +3643,13 @@
         <v>207</v>
       </c>
       <c r="E59" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F59" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G59" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3662,13 +3666,13 @@
         <v>208</v>
       </c>
       <c r="E60" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F60" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G60" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3685,13 +3689,13 @@
         <v>209</v>
       </c>
       <c r="E61" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F61" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G61" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3708,13 +3712,13 @@
         <v>210</v>
       </c>
       <c r="E62" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F62" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G62" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3731,13 +3735,13 @@
         <v>211</v>
       </c>
       <c r="E63" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F63" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G63" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3754,13 +3758,13 @@
         <v>212</v>
       </c>
       <c r="E64" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F64" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G64" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3777,13 +3781,13 @@
         <v>213</v>
       </c>
       <c r="E65" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F65" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G65" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3800,13 +3804,13 @@
         <v>214</v>
       </c>
       <c r="E66" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F66" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G66" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3820,16 +3824,16 @@
         <v>84</v>
       </c>
       <c r="D67" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E67" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F67" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G67" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3846,13 +3850,13 @@
         <v>215</v>
       </c>
       <c r="E68" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F68" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G68" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3869,13 +3873,13 @@
         <v>216</v>
       </c>
       <c r="E69" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F69" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G69" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3892,13 +3896,13 @@
         <v>217</v>
       </c>
       <c r="E70" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F70" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G70" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3915,13 +3919,13 @@
         <v>218</v>
       </c>
       <c r="E71" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F71" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G71" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3938,13 +3942,13 @@
         <v>219</v>
       </c>
       <c r="E72" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F72" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G72" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3961,13 +3965,13 @@
         <v>220</v>
       </c>
       <c r="E73" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F73" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G73" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3984,13 +3988,13 @@
         <v>221</v>
       </c>
       <c r="E74" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F74" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G74" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -4007,13 +4011,13 @@
         <v>222</v>
       </c>
       <c r="E75" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F75" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G75" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -4030,13 +4034,13 @@
         <v>223</v>
       </c>
       <c r="E76" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F76" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G76" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -4053,13 +4057,13 @@
         <v>224</v>
       </c>
       <c r="E77" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F77" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G77" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -4076,13 +4080,13 @@
         <v>225</v>
       </c>
       <c r="E78" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F78" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G78" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -4099,13 +4103,13 @@
         <v>226</v>
       </c>
       <c r="E79" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F79" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G79" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -4122,13 +4126,13 @@
         <v>227</v>
       </c>
       <c r="E80" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F80" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G80" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -4145,13 +4149,13 @@
         <v>228</v>
       </c>
       <c r="E81" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F81" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G81" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4168,13 +4172,13 @@
         <v>229</v>
       </c>
       <c r="E82" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F82" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G82" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -4191,13 +4195,13 @@
         <v>230</v>
       </c>
       <c r="E83" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F83" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G83" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4214,13 +4218,13 @@
         <v>231</v>
       </c>
       <c r="E84" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F84" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G84" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4237,13 +4241,13 @@
         <v>232</v>
       </c>
       <c r="E85" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F85" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G85" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4260,13 +4264,13 @@
         <v>233</v>
       </c>
       <c r="E86" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F86" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G86" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -4283,13 +4287,13 @@
         <v>234</v>
       </c>
       <c r="E87" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F87" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G87" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4306,13 +4310,13 @@
         <v>235</v>
       </c>
       <c r="E88" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F88" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G88" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -4329,13 +4333,13 @@
         <v>236</v>
       </c>
       <c r="E89" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F89" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G89" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -4352,13 +4356,13 @@
         <v>237</v>
       </c>
       <c r="E90" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F90" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G90" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -4375,13 +4379,13 @@
         <v>238</v>
       </c>
       <c r="E91" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F91" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G91" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -4398,13 +4402,13 @@
         <v>239</v>
       </c>
       <c r="E92" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F92" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G92" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -4421,13 +4425,13 @@
         <v>240</v>
       </c>
       <c r="E93" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F93" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G93" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -4444,13 +4448,13 @@
         <v>241</v>
       </c>
       <c r="E94" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F94" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G94" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -4467,13 +4471,13 @@
         <v>242</v>
       </c>
       <c r="E95" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F95" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G95" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -4490,13 +4494,13 @@
         <v>243</v>
       </c>
       <c r="E96" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F96" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G96" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -4513,13 +4517,13 @@
         <v>244</v>
       </c>
       <c r="E97" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F97" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G97" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -4533,16 +4537,16 @@
         <v>115</v>
       </c>
       <c r="D98" t="s">
-        <v>245</v>
+        <v>635</v>
       </c>
       <c r="E98" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F98" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G98" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -4556,16 +4560,16 @@
         <v>116</v>
       </c>
       <c r="D99" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E99" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F99" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G99" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -4579,16 +4583,16 @@
         <v>117</v>
       </c>
       <c r="D100" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E100" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F100" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G100" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -4602,16 +4606,16 @@
         <v>118</v>
       </c>
       <c r="D101" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E101" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F101" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G101" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -4625,16 +4629,16 @@
         <v>119</v>
       </c>
       <c r="D102" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E102" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F102" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G102" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -4648,16 +4652,16 @@
         <v>120</v>
       </c>
       <c r="D103" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E103" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F103" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G103" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -4671,16 +4675,16 @@
         <v>121</v>
       </c>
       <c r="D104" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E104" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F104" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G104" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -4694,16 +4698,16 @@
         <v>122</v>
       </c>
       <c r="D105" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E105" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F105" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G105" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -4717,16 +4721,16 @@
         <v>123</v>
       </c>
       <c r="D106" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E106" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F106" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G106" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4740,16 +4744,16 @@
         <v>124</v>
       </c>
       <c r="D107" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E107" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F107" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G107" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -4763,16 +4767,16 @@
         <v>125</v>
       </c>
       <c r="D108" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E108" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F108" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G108" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -4786,16 +4790,16 @@
         <v>126</v>
       </c>
       <c r="D109" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E109" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F109" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G109" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4809,16 +4813,16 @@
         <v>127</v>
       </c>
       <c r="D110" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E110" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F110" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G110" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4832,16 +4836,16 @@
         <v>128</v>
       </c>
       <c r="D111" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E111" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F111" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G111" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4855,16 +4859,16 @@
         <v>129</v>
       </c>
       <c r="D112" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E112" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F112" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G112" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4878,16 +4882,16 @@
         <v>130</v>
       </c>
       <c r="D113" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E113" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F113" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G113" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4901,16 +4905,16 @@
         <v>131</v>
       </c>
       <c r="D114" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E114" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F114" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G114" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4924,16 +4928,16 @@
         <v>132</v>
       </c>
       <c r="D115" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E115" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F115" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G115" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4947,16 +4951,16 @@
         <v>133</v>
       </c>
       <c r="D116" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E116" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F116" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G116" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -4970,16 +4974,16 @@
         <v>134</v>
       </c>
       <c r="D117" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E117" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F117" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G117" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -4993,16 +4997,16 @@
         <v>135</v>
       </c>
       <c r="D118" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E118" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F118" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G118" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -5016,16 +5020,16 @@
         <v>136</v>
       </c>
       <c r="D119" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E119" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F119" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G119" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -5039,16 +5043,16 @@
         <v>137</v>
       </c>
       <c r="D120" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E120" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F120" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G120" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -5062,16 +5066,16 @@
         <v>138</v>
       </c>
       <c r="D121" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E121" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F121" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G121" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -5085,16 +5089,16 @@
         <v>139</v>
       </c>
       <c r="D122" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E122" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F122" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G122" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -5108,16 +5112,16 @@
         <v>140</v>
       </c>
       <c r="D123" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E123" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F123" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G123" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -5131,16 +5135,16 @@
         <v>141</v>
       </c>
       <c r="D124" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E124" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F124" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G124" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -5154,16 +5158,16 @@
         <v>142</v>
       </c>
       <c r="D125" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E125" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F125" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G125" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -5177,16 +5181,16 @@
         <v>143</v>
       </c>
       <c r="D126" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E126" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F126" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G126" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -5200,16 +5204,16 @@
         <v>144</v>
       </c>
       <c r="D127" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E127" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F127" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G127" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -5223,16 +5227,16 @@
         <v>145</v>
       </c>
       <c r="D128" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E128" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F128" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G128" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -5245,17 +5249,17 @@
       <c r="C129" t="s">
         <v>146</v>
       </c>
-      <c r="D129" t="e">
-        <v>#N/A</v>
+      <c r="D129" t="s">
+        <v>634</v>
       </c>
       <c r="E129" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F129" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G129" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -5269,16 +5273,16 @@
         <v>147</v>
       </c>
       <c r="D130" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E130" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F130" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G130" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -5292,16 +5296,16 @@
         <v>148</v>
       </c>
       <c r="D131" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E131" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F131" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G131" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -5315,16 +5319,16 @@
         <v>149</v>
       </c>
       <c r="D132" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E132" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F132" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G132" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>